<commit_message>
Expanded the error-handling of the excel importer
</commit_message>
<xml_diff>
--- a/CluIt/excel/pixel_book.xlsx
+++ b/CluIt/excel/pixel_book.xlsx
@@ -363,50 +363,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A2:C173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="G165" sqref="G165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>-1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>-1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -417,7 +406,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -428,18 +417,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>-1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -450,7 +439,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -461,7 +450,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -472,7 +461,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -483,7 +472,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -494,29 +483,29 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>-1</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B13">
         <v>-1</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>-1</v>
@@ -527,7 +516,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>-1</v>
@@ -538,7 +527,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>-1</v>
@@ -549,7 +538,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>-1</v>
@@ -560,7 +549,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>-1</v>
@@ -571,18 +560,18 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>-1</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B20">
         <v>-1</v>
@@ -593,7 +582,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>-1</v>
@@ -604,7 +593,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>-1</v>
@@ -615,18 +604,18 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>-1</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>-1</v>
@@ -637,7 +626,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>-1</v>
@@ -648,7 +637,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>-1</v>
@@ -659,18 +648,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B27">
         <v>-1</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28">
         <v>-1</v>
@@ -681,7 +670,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>-1</v>
@@ -692,7 +681,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30">
         <v>-1</v>
@@ -703,7 +692,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B31">
         <v>-1</v>
@@ -714,18 +703,18 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>-1</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>-1</v>
@@ -736,7 +725,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B34">
         <v>-1</v>
@@ -747,7 +736,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B35">
         <v>-1</v>
@@ -758,18 +747,18 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B36">
         <v>-1</v>
       </c>
       <c r="C36">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>-1</v>
@@ -780,7 +769,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B38">
         <v>-1</v>
@@ -791,7 +780,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B39">
         <v>-1</v>
@@ -802,18 +791,18 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B40">
         <v>-1</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B41">
         <v>-1</v>
@@ -824,7 +813,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>-1</v>
@@ -835,7 +824,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <v>-1</v>
@@ -846,18 +835,18 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B44">
         <v>-1</v>
       </c>
       <c r="C44">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B45">
         <v>-1</v>
@@ -868,7 +857,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B46">
         <v>-1</v>
@@ -879,18 +868,18 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="B47">
         <v>-1</v>
       </c>
       <c r="C47">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B48">
         <v>-1</v>
@@ -901,7 +890,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B49">
         <v>-1</v>
@@ -912,7 +901,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B50">
         <v>-1</v>
@@ -923,7 +912,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51">
         <v>-1</v>
@@ -934,7 +923,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B52">
         <v>-1</v>
@@ -945,7 +934,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B53">
         <v>-1</v>
@@ -956,18 +945,18 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B54">
         <v>-1</v>
       </c>
       <c r="C54">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B55">
         <v>-1</v>
@@ -978,7 +967,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B56">
         <v>-1</v>
@@ -989,7 +978,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>-1</v>
@@ -1000,7 +989,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B58">
         <v>-1</v>
@@ -1011,7 +1000,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B59">
         <v>-1</v>
@@ -1022,18 +1011,18 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B60">
         <v>-1</v>
       </c>
       <c r="C60">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B61">
         <v>-1</v>
@@ -1044,7 +1033,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B62">
         <v>-1</v>
@@ -1055,7 +1044,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B63">
         <v>-1</v>
@@ -1066,18 +1055,18 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B64">
         <v>-1</v>
       </c>
       <c r="C64">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B65">
         <v>-1</v>
@@ -1088,7 +1077,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B66">
         <v>-1</v>
@@ -1099,7 +1088,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B67">
         <v>-1</v>
@@ -1110,18 +1099,18 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B68">
         <v>-1</v>
       </c>
       <c r="C68">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B69">
         <v>-1</v>
@@ -1132,7 +1121,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B70">
         <v>-1</v>
@@ -1143,7 +1132,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="B71">
         <v>-1</v>
@@ -1154,29 +1143,29 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B72">
         <v>-1</v>
       </c>
       <c r="C72">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B73">
         <v>-1</v>
       </c>
       <c r="C73">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B74">
         <v>-1</v>
@@ -1187,7 +1176,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B75">
         <v>-1</v>
@@ -1198,18 +1187,18 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B76">
         <v>-1</v>
       </c>
       <c r="C76">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B77">
         <v>-1</v>
@@ -1220,73 +1209,73 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B78">
         <v>-1</v>
       </c>
       <c r="C78">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B79">
         <v>-1</v>
       </c>
       <c r="C79">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B80">
         <v>-1</v>
       </c>
       <c r="C80">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B81">
         <v>-1</v>
       </c>
       <c r="C81">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B82">
         <v>-1</v>
       </c>
       <c r="C82">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B83">
         <v>-1</v>
       </c>
       <c r="C83">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>-1</v>
@@ -1297,18 +1286,18 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B85">
         <v>-1</v>
       </c>
       <c r="C85">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B86">
         <v>-1</v>
@@ -1319,7 +1308,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B87">
         <v>-1</v>
@@ -1330,18 +1319,18 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B88">
         <v>-1</v>
       </c>
       <c r="C88">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B89">
         <v>-1</v>
@@ -1352,7 +1341,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B90">
         <v>-1</v>
@@ -1363,7 +1352,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B91">
         <v>-1</v>
@@ -1374,7 +1363,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="B92">
         <v>-1</v>
@@ -1385,7 +1374,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B93">
         <v>-1</v>
@@ -1396,29 +1385,29 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B94">
         <v>-1</v>
       </c>
       <c r="C94">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B95">
         <v>-1</v>
       </c>
       <c r="C95">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B96">
         <v>-1</v>
@@ -1429,7 +1418,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B97">
         <v>-1</v>
@@ -1440,18 +1429,18 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B98">
         <v>-1</v>
       </c>
       <c r="C98">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B99">
         <v>-1</v>
@@ -1462,7 +1451,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="B100">
         <v>-1</v>
@@ -1473,18 +1462,18 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B101">
         <v>-1</v>
       </c>
       <c r="C101">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B102">
         <v>-1</v>
@@ -1495,18 +1484,18 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B103">
         <v>-1</v>
       </c>
       <c r="C103">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B104">
         <v>-1</v>
@@ -1517,7 +1506,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B105">
         <v>-1</v>
@@ -1528,18 +1517,18 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B106">
         <v>-1</v>
       </c>
       <c r="C106">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B107">
         <v>-1</v>
@@ -1550,18 +1539,18 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B108">
         <v>-1</v>
       </c>
       <c r="C108">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B109">
         <v>-1</v>
@@ -1572,18 +1561,18 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B110">
         <v>-1</v>
       </c>
       <c r="C110">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B111">
         <v>-1</v>
@@ -1594,7 +1583,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B112">
         <v>-1</v>
@@ -1605,18 +1594,18 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B113">
         <v>-1</v>
       </c>
       <c r="C113">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B114">
         <v>-1</v>
@@ -1627,7 +1616,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B115">
         <v>-1</v>
@@ -1638,7 +1627,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B116">
         <v>-1</v>
@@ -1649,18 +1638,18 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B117">
         <v>-1</v>
       </c>
       <c r="C117">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B118">
         <v>-1</v>
@@ -1671,7 +1660,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B119">
         <v>-1</v>
@@ -1682,7 +1671,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B120">
         <v>-1</v>
@@ -1693,18 +1682,18 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B121">
         <v>-1</v>
       </c>
       <c r="C121">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B122">
         <v>-1</v>
@@ -1715,7 +1704,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B123">
         <v>-1</v>
@@ -1726,18 +1715,18 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B124">
         <v>-1</v>
       </c>
       <c r="C124">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B125">
         <v>-1</v>
@@ -1748,7 +1737,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B126">
         <v>-1</v>
@@ -1759,7 +1748,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B127">
         <v>-1</v>
@@ -1770,7 +1759,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B128">
         <v>-1</v>
@@ -1781,18 +1770,18 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B129">
         <v>-1</v>
       </c>
       <c r="C129">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B130">
         <v>-1</v>
@@ -1803,7 +1792,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B131">
         <v>-1</v>
@@ -1814,7 +1803,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B132">
         <v>-1</v>
@@ -1825,7 +1814,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B133">
         <v>-1</v>
@@ -1836,18 +1825,18 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B134">
         <v>-1</v>
       </c>
       <c r="C134">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B135">
         <v>-1</v>
@@ -1858,7 +1847,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B136">
         <v>-1</v>
@@ -1869,18 +1858,18 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B137">
         <v>-1</v>
       </c>
       <c r="C137">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B138">
         <v>-1</v>
@@ -1891,7 +1880,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B139">
         <v>-1</v>
@@ -1902,7 +1891,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B140">
         <v>-1</v>
@@ -1913,18 +1902,18 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B141">
         <v>-1</v>
       </c>
       <c r="C141">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B142">
         <v>-1</v>
@@ -1935,7 +1924,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B143">
         <v>-1</v>
@@ -1946,18 +1935,18 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B144">
         <v>-1</v>
       </c>
       <c r="C144">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B145">
         <v>-1</v>
@@ -1968,7 +1957,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B146">
         <v>-1</v>
@@ -1979,18 +1968,18 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B147">
         <v>-1</v>
       </c>
       <c r="C147">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B148">
         <v>-1</v>
@@ -2001,7 +1990,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B149">
         <v>-1</v>
@@ -2012,18 +2001,18 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B150">
         <v>-1</v>
       </c>
       <c r="C150">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B151">
         <v>-1</v>
@@ -2034,7 +2023,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B152">
         <v>-1</v>
@@ -2045,7 +2034,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B153">
         <v>-1</v>
@@ -2056,18 +2045,18 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B154">
         <v>-1</v>
       </c>
       <c r="C154">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B155">
         <v>-1</v>
@@ -2078,7 +2067,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B156">
         <v>-1</v>
@@ -2089,29 +2078,29 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B157">
         <v>-1</v>
       </c>
       <c r="C157">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B158">
         <v>-1</v>
       </c>
       <c r="C158">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B159">
         <v>-1</v>
@@ -2122,7 +2111,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B160">
         <v>-1</v>
@@ -2133,18 +2122,18 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B161">
         <v>-1</v>
       </c>
       <c r="C161">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B162">
         <v>-1</v>
@@ -2155,18 +2144,18 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B163">
         <v>-1</v>
       </c>
       <c r="C163">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B164">
         <v>-1</v>
@@ -2177,18 +2166,18 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B165">
         <v>-1</v>
       </c>
       <c r="C165">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B166">
         <v>-1</v>
@@ -2199,7 +2188,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B167">
         <v>-1</v>
@@ -2210,7 +2199,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B168">
         <v>-1</v>
@@ -2221,7 +2210,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B169">
         <v>-1</v>
@@ -2232,34 +2221,45 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B170">
         <v>-1</v>
       </c>
       <c r="C170">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B171">
         <v>-1</v>
       </c>
       <c r="C171">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
+        <v>8</v>
+      </c>
+      <c r="B172">
+        <v>-1</v>
+      </c>
+      <c r="C172">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
         <v>21</v>
       </c>
-      <c r="B172">
-        <v>-1</v>
-      </c>
-      <c r="C172">
+      <c r="B173">
+        <v>-1</v>
+      </c>
+      <c r="C173">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for reference variables and normalization of data
</commit_message>
<xml_diff>
--- a/CluIt/excel/pixel_book.xlsx
+++ b/CluIt/excel/pixel_book.xlsx
@@ -365,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="F142" sqref="F142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B150">
         <v>-1</v>
@@ -2260,7 +2260,7 @@
         <v>-1</v>
       </c>
       <c r="C173">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>